<commit_message>
Add pdf of updated objectives
</commit_message>
<xml_diff>
--- a/Cycle_Two/HOQ and Specs SUBMISSION.xlsx
+++ b/Cycle_Two/HOQ and Specs SUBMISSION.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deepthinacharaju/Documents/Duke/Class/Fall 2018/BME590L/MediCall/Cycle_Two/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{418BF29C-57E5-C544-A4BE-80DE8D7342FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50DB93F-5683-7540-8E8B-C35B0D46BACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="940" windowWidth="27640" windowHeight="16120" xr2:uid="{20D96F55-8BA8-AF48-865C-6744F6B611E5}"/>
   </bookViews>
   <sheets>
     <sheet name="HOQ, Specs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -842,15 +847,15 @@
   </sheetPr>
   <dimension ref="A1:U1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13:W15"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="34.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="37.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="37.1640625" style="1" customWidth="1"/>

</xml_diff>